<commit_message>
🍱 Update some files
</commit_message>
<xml_diff>
--- a/tabellenliebe/00_Open_Data_Quellen.xlsx
+++ b/tabellenliebe/00_Open_Data_Quellen.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>https://open.nrw/open-data</t>
+  </si>
+  <si>
+    <t>Landesdatenbank NRW</t>
+  </si>
+  <si>
+    <t>https://www.landesdatenbank.nrw.de/</t>
   </si>
   <si>
     <t>Open Data Moers</t>
@@ -107,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -120,6 +126,11 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -142,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -154,6 +165,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -365,6 +382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -374,7 +392,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.57"/>
+    <col customWidth="1" min="1" max="1" width="40.14"/>
     <col customWidth="1" min="2" max="2" width="20.71"/>
     <col customWidth="1" min="3" max="3" width="49.57"/>
   </cols>
@@ -424,13 +442,13 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -461,29 +479,29 @@
         <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>25</v>
@@ -494,7 +512,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>27</v>
@@ -505,10 +523,21 @@
         <v>28</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +553,11 @@
     <hyperlink r:id="rId9" ref="C10"/>
     <hyperlink r:id="rId10" ref="C11"/>
     <hyperlink r:id="rId11" ref="C12"/>
+    <hyperlink r:id="rId12" ref="C13"/>
   </hyperlinks>
-  <drawing r:id="rId12"/>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
+  <drawing r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>